<commit_message>
added new set of trials
</commit_message>
<xml_diff>
--- a/Reliability Mesurements 1 mL Syringe Excel.xlsx
+++ b/Reliability Mesurements 1 mL Syringe Excel.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="9-2-14" sheetId="1" r:id="rId1"/>
+    <sheet name="9-3-14" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>Trial #</t>
   </si>
@@ -140,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -151,14 +152,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,11 +457,11 @@
     <col min="3" max="3" width="58.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -465,8 +469,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
@@ -560,22 +564,22 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
+      <c r="A12" s="5"/>
     </row>
     <row r="13" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
@@ -664,22 +668,22 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6"/>
+      <c r="A27" s="5"/>
     </row>
     <row r="28" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
       <c r="C29" s="2" t="s">
         <v>7</v>
       </c>
@@ -783,4 +787,114 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="43.5703125" customWidth="1"/>
+    <col min="3" max="3" width="58.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.20280000000000001</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.19939999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.2044</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.2001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.2014</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.19969999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.20039999999999999</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.19950000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.19620000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <f>(B3+B4+B5+B6+B7)/5</f>
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="C8" s="2">
+        <f>(C3+C5+C4+C6+C7)/5</f>
+        <v>0.19897999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>